<commit_message>
update readme and repo dependencies
</commit_message>
<xml_diff>
--- a/data/export/dqReports.xlsx
+++ b/data/export/dqReports.xlsx
@@ -8,10 +8,10 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="DQ Metrics" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Outliers" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="Contradictions" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="Missings" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="DQ_Metrics" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="DQ Metrics" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Outliers" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Contradictions" sheetId="4" state="visible" r:id="rId6"/>
     <sheet name="Semantics" sheetId="5" state="visible" r:id="rId7"/>
     <sheet name="RangeRules" sheetId="6" state="visible" r:id="rId8"/>
     <sheet name="LogicalRules" sheetId="7" state="visible" r:id="rId9"/>
@@ -63,7 +63,7 @@
     <t xml:space="preserve">Report Date (refers to the date of data export)</t>
   </si>
   <si>
-    <t xml:space="preserve">2025-03-02</t>
+    <t xml:space="preserve">2025-07-20</t>
   </si>
   <si>
     <t xml:space="preserve">dqi_co_icr</t>
@@ -72,7 +72,7 @@
     <t xml:space="preserve">Item Completeness Rate</t>
   </si>
   <si>
-    <t xml:space="preserve">97,73%</t>
+    <t xml:space="preserve">95,45%</t>
   </si>
   <si>
     <t xml:space="preserve">dqi_co_vcr</t>
@@ -81,7 +81,7 @@
     <t xml:space="preserve">Value Completeness Rate</t>
   </si>
   <si>
-    <t xml:space="preserve">99,36%</t>
+    <t xml:space="preserve">99,34%</t>
   </si>
   <si>
     <t xml:space="preserve">dqi_pl_rpr</t>
@@ -126,7 +126,7 @@
     <t xml:space="preserve">Mandatory Data Values</t>
   </si>
   <si>
-    <t xml:space="preserve">2021</t>
+    <t xml:space="preserve">1971</t>
   </si>
   <si>
     <t xml:space="preserve">im_misg</t>
@@ -135,7 +135,7 @@
     <t xml:space="preserve">Missing Mandatory Data Items</t>
   </si>
   <si>
-    <t xml:space="preserve">1</t>
+    <t xml:space="preserve">2</t>
   </si>
   <si>
     <t xml:space="preserve">vm_misg</t>
@@ -198,7 +198,7 @@
     <t xml:space="preserve">Execution Time</t>
   </si>
   <si>
-    <t xml:space="preserve">0.01</t>
+    <t xml:space="preserve">0</t>
   </si>
   <si>
     <t xml:space="preserve">mnppsd</t>
@@ -489,7 +489,7 @@
     <t xml:space="preserve">pseudo_02</t>
   </si>
   <si>
-    <t xml:space="preserve">Implausible time intervall according to the mathematical ruleMR3: basis_datum=2017-05-05, basis_gebdatum=2001-05-01, min=18years, max=130years </t>
+    <t xml:space="preserve">Implausible time interval according to the mathematical rule MR3: basis_datum=2017-05-05, basis_gebdatum=2001-05-01, min=18years, max=130years </t>
   </si>
   <si>
     <t xml:space="preserve">pseudo_06</t>
@@ -501,7 +501,7 @@
     <t xml:space="preserve">Implausible combination according to the mathematical rule MR1: basis_diastol=115, basis_systol=110 </t>
   </si>
   <si>
-    <t xml:space="preserve">Implausible time intervall according to the mathematical ruleMR6: basis_exrauch=2019-01-01, basis_datum=2017-05-05, min=NAdays, max=0days </t>
+    <t xml:space="preserve">Implausible time interval according to the mathematical rule MR6: basis_exrauch=2019-01-01, basis_datum=2017-05-05, min=NAdays, max=0days </t>
   </si>
   <si>
     <t xml:space="preserve">Implausible combination according to the logical rule LR3: basis_khk=nein, basis_bypass=ja </t>
@@ -510,7 +510,7 @@
     <t xml:space="preserve">Implausible combination according to the logical rule LR3: basis_khk=nein, basis_bypass=ja</t>
   </si>
   <si>
-    <t xml:space="preserve">Implausible time intervall according to the mathematical ruleMR2: basis_datum=2017-05-20, basis_datum_blut=2017-04-27, min=-7days, max=7days </t>
+    <t xml:space="preserve">Implausible time interval according to the mathematical rule MR2: basis_datum=2017-05-20, basis_datum_blut=2017-04-27, min=-7days, max=7days </t>
   </si>
   <si>
     <t xml:space="preserve">missing_values</t>
@@ -522,7 +522,7 @@
     <t xml:space="preserve">Missing value for basis_exrauch according to the missing rule MR2 for hideable data values </t>
   </si>
   <si>
-    <t xml:space="preserve">missing  basis_diabetes according to the list of mandatory metadata  </t>
+    <t xml:space="preserve">missing  basis_diabetes according to the list of mandatory metadata  missing  basis_ethni according to the list of mandatory metadata  </t>
   </si>
   <si>
     <t xml:space="preserve">pseudo_17</t>
@@ -899,11 +899,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1101,7 +1101,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1339,15 +1339,15 @@
   </sheetPr>
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="61.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="53.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="13.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.71"/>
@@ -1906,15 +1906,15 @@
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="61.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="51.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="143.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="6" style="1" width="9.15"/>
@@ -2142,18 +2142,17 @@
   </sheetPr>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="61.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="52.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="91.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="69.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="81.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="135.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="7" style="1" width="9.15"/>
   </cols>
   <sheetData>
@@ -2456,14 +2455,14 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="175.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="5" style="1" width="9.15"/>
   </cols>
@@ -2564,8 +2563,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="7.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.71"/>
@@ -3167,7 +3165,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3179,7 +3177,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="5.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="4.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="9" style="1" width="9.15"/>
   </cols>
   <sheetData>

</xml_diff>